<commit_message>
rechtzetting fout gebied onbekend streekwerking
</commit_message>
<xml_diff>
--- a/data_voor_swing/aggregatietabellen/streekwerking_provincie.xlsx
+++ b/data_voor_swing/aggregatietabellen/streekwerking_provincie.xlsx
@@ -1,40 +1,119 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr showObjects="all" updateLinks="userSet" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\gebiedsniveaus\data_voor_swing\aggregatietabellen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5C136B-9FAD-4D7B-A3A0-E3E2CBFC7534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" xWindow="480" yWindow="75" windowWidth="18075" windowHeight="12525" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="streekwerking_provincie" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="streekwerking_provincie" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="auto" refMode="A1" iterateCount="100"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>streekwerking</t>
+  </si>
+  <si>
+    <t>provincie</t>
+  </si>
+  <si>
+    <t>sw01</t>
+  </si>
+  <si>
+    <t>sw02</t>
+  </si>
+  <si>
+    <t>sw03</t>
+  </si>
+  <si>
+    <t>sw04</t>
+  </si>
+  <si>
+    <t>sw05</t>
+  </si>
+  <si>
+    <t>sw11</t>
+  </si>
+  <si>
+    <t>sw12</t>
+  </si>
+  <si>
+    <t>sw13</t>
+  </si>
+  <si>
+    <t>sw14</t>
+  </si>
+  <si>
+    <t>sw15</t>
+  </si>
+  <si>
+    <t>sw16</t>
+  </si>
+  <si>
+    <t>sw21</t>
+  </si>
+  <si>
+    <t>sw22</t>
+  </si>
+  <si>
+    <t>sw23</t>
+  </si>
+  <si>
+    <t>sw24</t>
+  </si>
+  <si>
+    <t>sw25</t>
+  </si>
+  <si>
+    <t>sw26</t>
+  </si>
+  <si>
+    <t>sw31</t>
+  </si>
+  <si>
+    <t>sw32</t>
+  </si>
+  <si>
+    <t>sw33</t>
+  </si>
+  <si>
+    <t>sw34</t>
+  </si>
+  <si>
+    <t>sw35</t>
+  </si>
+  <si>
+    <t>sw36</t>
+  </si>
+  <si>
+    <t>sw41</t>
+  </si>
+  <si>
+    <t>sw91</t>
+  </si>
+  <si>
+    <t>sw93</t>
+  </si>
+  <si>
+    <t>sw99</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="17">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000"/>
-    <numFmt numFmtId="172" formatCode="0.00000000"/>
-    <numFmt numFmtId="173" formatCode="0.000000000"/>
-    <numFmt numFmtId="174" formatCode="0.0000000000"/>
-    <numFmt numFmtId="175" formatCode="0.00000000000"/>
-    <numFmt numFmtId="176" formatCode="0.000000000000"/>
-    <numFmt numFmtId="177" formatCode="0.0000000000000"/>
-    <numFmt numFmtId="178" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="179" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="180" formatCode="0.0000000000000000"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,44 +142,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -138,7 +203,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -172,6 +237,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -206,9 +272,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -381,292 +448,236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="0" outlineLevel="0">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>streekwerking</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>provincie</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="0" outlineLevel="0">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>sw01</t>
-        </is>
-      </c>
-      <c r="B2" s="23">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
         <v>20001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="0" outlineLevel="0">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>sw02</t>
-        </is>
-      </c>
-      <c r="B3" s="23">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
         <v>20001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="0" outlineLevel="0">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>sw03</t>
-        </is>
-      </c>
-      <c r="B4" s="23">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
         <v>20001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="0" outlineLevel="0">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>sw04</t>
-        </is>
-      </c>
-      <c r="B5" s="23">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
         <v>20001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="0" outlineLevel="0">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>sw05</t>
-        </is>
-      </c>
-      <c r="B6" s="23">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
         <v>20001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="0" outlineLevel="0">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>sw11</t>
-        </is>
-      </c>
-      <c r="B7" s="23">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="0" outlineLevel="0">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>sw12</t>
-        </is>
-      </c>
-      <c r="B8" s="23">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="0" outlineLevel="0">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>sw13</t>
-        </is>
-      </c>
-      <c r="B9" s="23">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="0" outlineLevel="0">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>sw14</t>
-        </is>
-      </c>
-      <c r="B10" s="23">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="0" outlineLevel="0">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>sw15</t>
-        </is>
-      </c>
-      <c r="B11" s="23">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="0" outlineLevel="0">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>sw16</t>
-        </is>
-      </c>
-      <c r="B12" s="23">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="0" outlineLevel="0">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>sw21</t>
-        </is>
-      </c>
-      <c r="B13" s="23">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
         <v>30000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="0" outlineLevel="0">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>sw22</t>
-        </is>
-      </c>
-      <c r="B14" s="23">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
         <v>30000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="0" outlineLevel="0">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>sw23</t>
-        </is>
-      </c>
-      <c r="B15" s="23">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
         <v>30000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="0" outlineLevel="0">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>sw24</t>
-        </is>
-      </c>
-      <c r="B16" s="23">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
         <v>30000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="0" outlineLevel="0">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>sw25</t>
-        </is>
-      </c>
-      <c r="B17" s="23">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
         <v>30000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="0" outlineLevel="0">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>sw26</t>
-        </is>
-      </c>
-      <c r="B18" s="23">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1">
         <v>30000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="0" outlineLevel="0">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>sw31</t>
-        </is>
-      </c>
-      <c r="B19" s="23">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="0" outlineLevel="0">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>sw32</t>
-        </is>
-      </c>
-      <c r="B20" s="23">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="0" outlineLevel="0">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>sw33</t>
-        </is>
-      </c>
-      <c r="B21" s="23">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="0" outlineLevel="0">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>sw34</t>
-        </is>
-      </c>
-      <c r="B22" s="23">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="0" outlineLevel="0">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>sw35</t>
-        </is>
-      </c>
-      <c r="B23" s="23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="0" outlineLevel="0">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>sw36</t>
-        </is>
-      </c>
-      <c r="B24" s="23">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="0" outlineLevel="0">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>sw41</t>
-        </is>
-      </c>
-      <c r="B25" s="23">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1">
         <v>70000</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="0" outlineLevel="0">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>sw91</t>
-        </is>
-      </c>
-      <c r="B26" s="23">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1">
         <v>99991</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="0" outlineLevel="0">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>sw93</t>
-        </is>
-      </c>
-      <c r="B27" s="23">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1">
         <v>99993</v>
       </c>
     </row>
-    <row r="28" spans="1:2" s="0" outlineLevel="0">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>sw93</t>
-        </is>
-      </c>
-      <c r="B28" s="23">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1">
         <v>99999</v>
       </c>
     </row>

</xml_diff>